<commit_message>
Test case number 5 is passing tests! The side multicolumn version of the test case haven't been implemented yet.
Signed-off-by: Agustín Benassi <agusbenassi@gmail.com>
</commit_message>
<xml_diff>
--- a/tests/integration_cases/expected/test_case5.xlsx
+++ b/tests/integration_cases/expected/test_case5.xlsx
@@ -16,10 +16,10 @@
     <t>datetime</t>
   </si>
   <si>
-    <t>RESERVAS INTERNACIONALES DEL B.C.R.A (1)., en millones de dolares                                            Oro, divisas, colocaciones a plazo y otros - Saldos</t>
+    <t>Saldos</t>
   </si>
   <si>
-    <t>RESERVAS INTERNACIONALES DEL B.C.R.A (1)., en millones de dolares                                            Oro, divisas, colocaciones a plazo y otros - Promedio mensual de saldos diarios</t>
+    <t>Promedio mensual de saldos diarios</t>
   </si>
 </sst>
 </file>
@@ -29,7 +29,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -43,10 +43,15 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Arial"/>
+      <name val="Verdana"/>
     </font>
     <font>
       <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
@@ -171,42 +176,42 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="4" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="4" fontId="4" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>

</xml_diff>